<commit_message>
used python script to generate probabilities
</commit_message>
<xml_diff>
--- a/tests/TI_Fonte.xlsx
+++ b/tests/TI_Fonte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSIDADE_STUFF\UNI\3a\1s\TI\TI_GROUP_WORK\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451009DD-B602-4273-B4E4-A132479EEF16}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B36856-5800-4250-9ABE-6FD04F16D05B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2AACDE5C-D3A9-4C50-8E15-7E551BEA9752}"/>
+    <workbookView xWindow="6120" yWindow="1395" windowWidth="21600" windowHeight="11385" activeTab="11" xr2:uid="{2AACDE5C-D3A9-4C50-8E15-7E551BEA9752}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -477,15 +477,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45B7ECBC-F3BB-4FC2-8C87-2B486545B693}" name="Table2" displayName="Table2" ref="A1:F6" totalsRowShown="0" headerRowDxfId="32" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45B7ECBC-F3BB-4FC2-8C87-2B486545B693}" name="Table2" displayName="Table2" ref="A1:F6" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A1:F6" xr:uid="{5497B681-3AD8-44F9-8D9D-6D02DE7839E0}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{AF9129D3-2D60-47F8-B33D-0CD5D3446CB1}" name="Column1" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{90716298-F419-4D0B-9CF0-1B878C1656F8}" name="1" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{1FDB1C13-BECB-47AD-8F9C-8081E9D0A1CE}" name="2" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{ADC627C2-3263-4B57-A6CE-D82B94C826E3}" name="3" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{9F2C0C13-D64B-4FF2-8F48-62FFAECF1CA7}" name="4" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{5236973C-975C-46A4-AB14-5E815C2E5A96}" name="Total" dataDxfId="34">
+    <tableColumn id="1" xr3:uid="{AF9129D3-2D60-47F8-B33D-0CD5D3446CB1}" name="Column1" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{90716298-F419-4D0B-9CF0-1B878C1656F8}" name="1" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{1FDB1C13-BECB-47AD-8F9C-8081E9D0A1CE}" name="2" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{ADC627C2-3263-4B57-A6CE-D82B94C826E3}" name="3" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{9F2C0C13-D64B-4FF2-8F48-62FFAECF1CA7}" name="4" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{5236973C-975C-46A4-AB14-5E815C2E5A96}" name="Total" dataDxfId="40">
       <calculatedColumnFormula>SUM(B2:E2)/4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -494,15 +494,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FCF6600-77A1-477C-9578-38E5455F0D9C}" name="Table1" displayName="Table1" ref="A1:F4" totalsRowShown="0" headerRowDxfId="40" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FCF6600-77A1-477C-9578-38E5455F0D9C}" name="Table1" displayName="Table1" ref="A1:F4" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A1:F4" xr:uid="{E09147CD-8B2D-4AD9-A5C8-68F0841B7A9B}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B3E47F96-6B4F-4D9E-B833-645C8721F0CC}" name="Column1" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{A85180D1-72E5-4F0E-8B1A-963DB3EBFBC8}" name="1" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{02643A54-F158-4DE4-AD33-EA62B28D3836}" name="2" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{EF79131F-7236-476C-AB77-521818DA2D59}" name="3" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{5ACC58FA-39F5-4E4B-A356-A27439658C48}" name="4" dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{B681919E-F5AE-47C6-ADD9-A141148FBC55}" name="Total" dataDxfId="42">
+    <tableColumn id="1" xr3:uid="{B3E47F96-6B4F-4D9E-B833-645C8721F0CC}" name="Column1" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{A85180D1-72E5-4F0E-8B1A-963DB3EBFBC8}" name="1" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{02643A54-F158-4DE4-AD33-EA62B28D3836}" name="2" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{EF79131F-7236-476C-AB77-521818DA2D59}" name="3" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{5ACC58FA-39F5-4E4B-A356-A27439658C48}" name="4" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{B681919E-F5AE-47C6-ADD9-A141148FBC55}" name="Total" dataDxfId="32">
       <calculatedColumnFormula>SUM(B2:E2)/4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471C816F-CD6F-46D1-BDDC-D33DDCE112A3}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,11 +1642,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3DFA79-9423-4F2E-9A23-DB8C6AA60AC6}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1672,26 +1675,42 @@
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="B2" s="1">
+        <v>8993</v>
+      </c>
+      <c r="C2" s="1">
+        <v>8968</v>
+      </c>
+      <c r="D2" s="1">
+        <v>8978</v>
+      </c>
+      <c r="E2" s="1">
+        <v>9017</v>
+      </c>
       <c r="F2" s="1">
         <f>SUM(B2:E2)/4</f>
-        <v>0</v>
+        <v>8989</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="B3" s="1">
+        <v>25936</v>
+      </c>
+      <c r="C3" s="1">
+        <v>25455</v>
+      </c>
+      <c r="D3" s="1">
+        <v>26091</v>
+      </c>
+      <c r="E3" s="1">
+        <v>26365</v>
+      </c>
       <c r="F3" s="1">
         <f>SUM(B3:E3)/4</f>
-        <v>0</v>
+        <v>25961.75</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1699,74 +1718,74 @@
         <v>17</v>
       </c>
       <c r="B4" s="1">
-        <f>SUM(B3:B3)</f>
-        <v>0</v>
+        <f>SUM(B2:B3)</f>
+        <v>34929</v>
       </c>
       <c r="C4" s="1">
-        <f>SUM(C3:C3)</f>
-        <v>0</v>
+        <f t="shared" ref="C4:E4" si="0">SUM(C2:C3)</f>
+        <v>34423</v>
       </c>
       <c r="D4" s="1">
-        <f>SUM(D3:D3)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>35069</v>
       </c>
       <c r="E4" s="1">
-        <f>SUM(E3:E3)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>35382</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F5" si="0">SUM(B4:E4)/4</f>
-        <v>0</v>
+        <f t="shared" ref="F4:F5" si="1">SUM(B4:E4)/4</f>
+        <v>34950.75</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="1" t="e">
-        <f>B3/B4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C5" s="1" t="e">
-        <f>C3/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D5" s="1" t="e">
-        <f>D3/D4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E5" s="1" t="e">
-        <f>E3/E4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F5" s="13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B5" s="1">
+        <f>B2/B4</f>
+        <v>0.25746514357697042</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ref="C5:E5" si="2">C2/C4</f>
+        <v>0.26052348720332336</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.256009581111523</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.25484709739415523</v>
+      </c>
+      <c r="F5" s="13">
+        <f t="shared" si="1"/>
+        <v>0.25721132732149299</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="1" t="e">
-        <f>B4/B5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" s="1" t="e">
-        <f>C4/C5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" s="1" t="e">
-        <f>D4/D5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" s="1" t="e">
-        <f>E4/E5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F6" s="13" t="e">
-        <f t="shared" ref="F6" si="1">SUM(B6:E6)/4</f>
-        <v>#DIV/0!</v>
+      <c r="B6" s="1">
+        <f>B3/B4</f>
+        <v>0.74253485642302952</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ref="C6:E6" si="3">C3/C4</f>
+        <v>0.73947651279667659</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="3"/>
+        <v>0.74399041888847706</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="3"/>
+        <v>0.74515290260584477</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" ref="F6" si="4">SUM(B6:E6)/4</f>
+        <v>0.74278867267850701</v>
       </c>
     </row>
   </sheetData>
@@ -2023,8 +2042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA30243-74B1-46F8-AE5B-6E8588B163F2}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A4" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2446,8 +2465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6F8EFB-283B-4BDF-BB77-AD38B2BA8333}">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A4" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3511,7 +3530,7 @@
         <v>3171</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:F4" si="1">SUM(C2:C3)</f>
+        <f t="shared" ref="C4:E4" si="1">SUM(C2:C3)</f>
         <v>3280</v>
       </c>
       <c r="D4" s="1">
@@ -3681,7 +3700,7 @@
         <v>983</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F5" si="0">SUM(B3:E3)/4</f>
+        <f t="shared" ref="F3:F4" si="0">SUM(B3:E3)/4</f>
         <v>1011</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added missing probabilities to the all sheet
</commit_message>
<xml_diff>
--- a/tests/TI_Fonte.xlsx
+++ b/tests/TI_Fonte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSIDADE_STUFF\UNI\3a\1s\TI\TI_GROUP_WORK\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B36856-5800-4250-9ABE-6FD04F16D05B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8E8ECD-58A1-4F8E-B146-43451C9D37DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="1395" windowWidth="21600" windowHeight="11385" activeTab="11" xr2:uid="{2AACDE5C-D3A9-4C50-8E15-7E551BEA9752}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2AACDE5C-D3A9-4C50-8E15-7E551BEA9752}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -258,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -296,6 +296,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -877,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471C816F-CD6F-46D1-BDDC-D33DDCE112A3}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,7 +958,10 @@
       <c r="K2" s="3">
         <v>0</v>
       </c>
-      <c r="L2" s="12"/>
+      <c r="L2" s="12">
+        <f>'-'!F5</f>
+        <v>0.25721132732149299</v>
+      </c>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1362,7 +1368,10 @@
       <c r="K12" s="3">
         <v>0</v>
       </c>
-      <c r="L12" s="12"/>
+      <c r="L12" s="15">
+        <f>'-'!F6</f>
+        <v>0.74278867267850701</v>
+      </c>
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1411,7 +1420,7 @@
       </c>
       <c r="L13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="1"/>
     </row>
@@ -1642,8 +1651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3DFA79-9423-4F2E-9A23-DB8C6AA60AC6}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>